<commit_message>
corrected beam element stiffness matrix (in fem_classes). Correction fixes results for beam and beam/truss models in ./test
</commit_message>
<xml_diff>
--- a/test/output.xlsx
+++ b/test/output.xlsx
@@ -345,30 +345,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:15">
       <c r="A1">
-        <v>99.9999999936</v>
+        <v>1600</v>
       </c>
       <c r="B1">
-        <v>1.218523565152008E-12</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>-249.999999984</v>
+        <v>0</v>
       </c>
       <c r="D1">
-        <v>-99.9999999936</v>
+        <v>-1600</v>
       </c>
       <c r="E1">
-        <v>-1.218523565152008E-12</v>
+        <v>0</v>
       </c>
       <c r="F1">
-        <v>-249.999999984</v>
+        <v>0</v>
       </c>
       <c r="G1">
         <v>0</v>
@@ -388,25 +388,34 @@
       <c r="L1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
-        <v>1.218523565152008E-12</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>20000</v>
+        <v>13.65333333333334</v>
       </c>
       <c r="C2">
-        <v>1.53080849883622E-14</v>
+        <v>5120</v>
       </c>
       <c r="D2">
-        <v>-1.218523565152008E-12</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>-20000</v>
+        <v>-13.65333333333334</v>
       </c>
       <c r="F2">
-        <v>1.53080849883622E-14</v>
+        <v>5120</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -426,25 +435,34 @@
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
-        <v>-249.999999984</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>1.530808498836219E-14</v>
+        <v>5120</v>
       </c>
       <c r="C3">
-        <v>833.33333328</v>
+        <v>2560000</v>
       </c>
       <c r="D3">
-        <v>249.999999984</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>-1.530808498836219E-14</v>
+        <v>-5120</v>
       </c>
       <c r="F3">
-        <v>416.66666664</v>
+        <v>1280000</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -464,31 +482,40 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
-        <v>-99.9999999936</v>
+        <v>-1600</v>
       </c>
       <c r="B4">
-        <v>-1.218523565152008E-12</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>-249.999999984</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>20099.9999999936</v>
+        <v>1750.000001474839</v>
       </c>
       <c r="E4">
-        <v>1.218523565152008E-12</v>
+        <v>-259.807622554496</v>
       </c>
       <c r="F4">
-        <v>249.999999984</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>-20000</v>
+        <v>-150.0000014748388</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>259.807622554496</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -502,34 +529,43 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
-        <v>-1.218523565152008E-12</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>-20000</v>
+        <v>-13.65333333333334</v>
       </c>
       <c r="C5">
-        <v>1.53080849883622E-14</v>
+        <v>-5120</v>
       </c>
       <c r="D5">
-        <v>1.218523565152008E-12</v>
+        <v>-259.8076225544959</v>
       </c>
       <c r="E5">
-        <v>20099.9999999936</v>
+        <v>463.6533338249466</v>
       </c>
       <c r="F5">
-        <v>249.9999999839999</v>
+        <v>-5120</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>259.8076225544959</v>
       </c>
       <c r="H5">
-        <v>-99.9999999936</v>
+        <v>-450.0000004916132</v>
       </c>
       <c r="I5">
-        <v>249.999999984</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -540,34 +576,43 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
-        <v>249.999999984</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>-1.530808498836219E-14</v>
+        <v>5120</v>
       </c>
       <c r="C6">
-        <v>416.66666664</v>
+        <v>1280000</v>
       </c>
       <c r="D6">
-        <v>249.999999984</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>249.9999999839999</v>
+        <v>-5120</v>
       </c>
       <c r="F6">
-        <v>1666.66666656</v>
+        <v>2560000</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>-249.999999984</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>416.66666664</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -578,8 +623,17 @@
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>0</v>
       </c>
@@ -590,34 +644,43 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>-20000</v>
+        <v>-150.0000014748388</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>259.807622554496</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>20099.9999999936</v>
+        <v>222.0000014748388</v>
       </c>
       <c r="H7">
-        <v>3.655570695456025E-12</v>
+        <v>-259.8076225544958</v>
       </c>
       <c r="I7">
-        <v>249.999999984</v>
+        <v>-18000</v>
       </c>
       <c r="J7">
-        <v>-99.9999999936</v>
+        <v>-72.00000000000001</v>
       </c>
       <c r="K7">
-        <v>-3.655570695456025E-12</v>
+        <v>-1.792882913951725E-13</v>
       </c>
       <c r="L7">
-        <v>249.999999984</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>-18000</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>0</v>
       </c>
@@ -628,34 +691,43 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>259.8076225544959</v>
       </c>
       <c r="E8">
-        <v>-99.9999999936</v>
+        <v>-450.0000004916132</v>
       </c>
       <c r="F8">
-        <v>249.999999984</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>3.655570695456025E-12</v>
+        <v>-259.8076225544958</v>
       </c>
       <c r="H8">
-        <v>20099.9999999936</v>
+        <v>3450.000000491613</v>
       </c>
       <c r="I8">
-        <v>-249.999999984</v>
+        <v>1.102182119232618E-12</v>
       </c>
       <c r="J8">
-        <v>-3.655570695456025E-12</v>
+        <v>-1.792882913951725E-13</v>
       </c>
       <c r="K8">
-        <v>-20000</v>
+        <v>-3000</v>
       </c>
       <c r="L8">
-        <v>-4.592425496508659E-14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>1.102182119232618E-12</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>0</v>
       </c>
@@ -669,31 +741,40 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>-249.999999984</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>416.66666664</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>249.999999984</v>
+        <v>-18000</v>
       </c>
       <c r="H9">
-        <v>-249.999999984</v>
+        <v>1.102182119232618E-12</v>
       </c>
       <c r="I9">
-        <v>1666.66666656</v>
+        <v>6000000</v>
       </c>
       <c r="J9">
-        <v>-249.999999984</v>
+        <v>18000</v>
       </c>
       <c r="K9">
-        <v>4.592425496508659E-14</v>
+        <v>-1.102182119232618E-12</v>
       </c>
       <c r="L9">
-        <v>416.66666664</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>3000000</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>0</v>
       </c>
@@ -713,25 +794,34 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>-99.9999999936</v>
+        <v>-72.00000000000001</v>
       </c>
       <c r="H10">
-        <v>-3.655570695456025E-12</v>
+        <v>-1.792882913951725E-13</v>
       </c>
       <c r="I10">
-        <v>249.999999984</v>
+        <v>18000</v>
       </c>
       <c r="J10">
-        <v>99.9999999936</v>
+        <v>81.00000000000001</v>
       </c>
       <c r="K10">
-        <v>3.655570695456025E-12</v>
+        <v>2.705857102716078E-13</v>
       </c>
       <c r="L10">
-        <v>-249.999999984</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>13500</v>
+      </c>
+      <c r="M10">
+        <v>-9.000000000000002</v>
+      </c>
+      <c r="N10">
+        <v>-9.129741887643519E-14</v>
+      </c>
+      <c r="O10">
+        <v>-4500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>0</v>
       </c>
@@ -751,25 +841,34 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>-3.655570695456025E-12</v>
+        <v>-1.792882913951725E-13</v>
       </c>
       <c r="H11">
-        <v>-20000</v>
+        <v>-3000</v>
       </c>
       <c r="I11">
-        <v>-4.592425496508659E-14</v>
+        <v>-1.102182119232618E-12</v>
       </c>
       <c r="J11">
-        <v>3.655570695456025E-12</v>
+        <v>2.705857102716077E-13</v>
       </c>
       <c r="K11">
-        <v>20000</v>
+        <v>4500</v>
       </c>
       <c r="L11">
-        <v>4.592425496508659E-14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>-8.266365894244634E-13</v>
+      </c>
+      <c r="M11">
+        <v>-9.129741887643518E-14</v>
+      </c>
+      <c r="N11">
+        <v>-1500</v>
+      </c>
+      <c r="O11">
+        <v>2.755455298081545E-13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>0</v>
       </c>
@@ -789,22 +888,172 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>-249.999999984</v>
+        <v>-18000</v>
       </c>
       <c r="H12">
-        <v>4.592425496508659E-14</v>
+        <v>1.102182119232618E-12</v>
       </c>
       <c r="I12">
-        <v>416.66666664</v>
+        <v>3000000</v>
       </c>
       <c r="J12">
-        <v>-249.999999984</v>
+        <v>13500</v>
       </c>
       <c r="K12">
-        <v>4.592425496508659E-14</v>
+        <v>-8.266365894244634E-13</v>
       </c>
       <c r="L12">
-        <v>833.33333328</v>
+        <v>9000000</v>
+      </c>
+      <c r="M12">
+        <v>4500</v>
+      </c>
+      <c r="N12">
+        <v>-2.755455298081545E-13</v>
+      </c>
+      <c r="O12">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>-9.000000000000002</v>
+      </c>
+      <c r="K13">
+        <v>-9.129741887643519E-14</v>
+      </c>
+      <c r="L13">
+        <v>4500</v>
+      </c>
+      <c r="M13">
+        <v>9.000000000000002</v>
+      </c>
+      <c r="N13">
+        <v>9.129741887643519E-14</v>
+      </c>
+      <c r="O13">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>-9.129741887643518E-14</v>
+      </c>
+      <c r="K14">
+        <v>-1500</v>
+      </c>
+      <c r="L14">
+        <v>-2.755455298081545E-13</v>
+      </c>
+      <c r="M14">
+        <v>9.129741887643518E-14</v>
+      </c>
+      <c r="N14">
+        <v>1500</v>
+      </c>
+      <c r="O14">
+        <v>-2.755455298081545E-13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>-4500</v>
+      </c>
+      <c r="K15">
+        <v>2.755455298081545E-13</v>
+      </c>
+      <c r="L15">
+        <v>1500000</v>
+      </c>
+      <c r="M15">
+        <v>4500</v>
+      </c>
+      <c r="N15">
+        <v>-2.755455298081545E-13</v>
+      </c>
+      <c r="O15">
+        <v>3000000</v>
       </c>
     </row>
   </sheetData>
@@ -814,7 +1063,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -837,17 +1086,17 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>-25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>-20.83333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -857,12 +1106,12 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>-25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>20.83333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -877,6 +1126,21 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
         <v>0</v>
       </c>
     </row>
@@ -887,7 +1151,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -910,32 +1174,32 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>0.7159879926484235</v>
+        <v>0.01250000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>0.0008878368024535339</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>-0.1029687141757193</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>0.7132808236843223</v>
+        <v>-1.566217468152431</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>-0.0008136189482254767</v>
+        <v>0.01154700533333348</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>-0.06873881233178429</v>
+        <v>-0.004243546047415973</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -950,7 +1214,22 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>0</v>
+        <v>-0.0009102127140826424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>-3.534231730361798</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>2.160010632019136E-16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>0.005756453952584019</v>
       </c>
     </row>
   </sheetData>
@@ -960,24 +1239,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1">
-        <v>20099.9999999936</v>
+        <v>1750.000001474839</v>
       </c>
       <c r="B1">
-        <v>1.218523565152008E-12</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>249.999999984</v>
+        <v>-150.0000014748388</v>
       </c>
       <c r="D1">
-        <v>-20000</v>
+        <v>259.807622554496</v>
       </c>
       <c r="E1">
         <v>0</v>
@@ -985,105 +1264,246 @@
       <c r="F1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
-        <v>1.218523565152008E-12</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>20099.9999999936</v>
+        <v>2560000</v>
       </c>
       <c r="C2">
-        <v>249.9999999839999</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>-99.9999999936</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>249.999999984</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
-        <v>249.999999984</v>
+        <v>-150.0000014748388</v>
       </c>
       <c r="B3">
-        <v>249.9999999839999</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1666.66666656</v>
+        <v>222.0000014748388</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>-259.8076225544958</v>
       </c>
       <c r="E3">
-        <v>-249.999999984</v>
+        <v>-18000</v>
       </c>
       <c r="F3">
-        <v>416.66666664</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>-18000</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
-        <v>-20000</v>
+        <v>259.8076225544959</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-259.8076225544958</v>
       </c>
       <c r="D4">
-        <v>20099.9999999936</v>
+        <v>3450.000000491613</v>
       </c>
       <c r="E4">
-        <v>3.655570695456025E-12</v>
+        <v>1.102182119232618E-12</v>
       </c>
       <c r="F4">
-        <v>249.999999984</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>1.102182119232618E-12</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
-        <v>-99.9999999936</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>249.999999984</v>
+        <v>-18000</v>
       </c>
       <c r="D5">
-        <v>3.655570695456025E-12</v>
+        <v>1.102182119232618E-12</v>
       </c>
       <c r="E5">
-        <v>20099.9999999936</v>
+        <v>6000000</v>
       </c>
       <c r="F5">
-        <v>-249.999999984</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>3000000</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="B6">
-        <v>-249.999999984</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>416.66666664</v>
+        <v>-18000</v>
       </c>
       <c r="D6">
-        <v>249.999999984</v>
+        <v>1.102182119232618E-12</v>
       </c>
       <c r="E6">
-        <v>-249.999999984</v>
+        <v>3000000</v>
       </c>
       <c r="F6">
-        <v>1666.66666656</v>
+        <v>9000000</v>
+      </c>
+      <c r="G6">
+        <v>4500</v>
+      </c>
+      <c r="H6">
+        <v>-2.755455298081545E-13</v>
+      </c>
+      <c r="I6">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>4500</v>
+      </c>
+      <c r="G7">
+        <v>9.000000000000002</v>
+      </c>
+      <c r="H7">
+        <v>9.129741887643519E-14</v>
+      </c>
+      <c r="I7">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>-2.755455298081545E-13</v>
+      </c>
+      <c r="G8">
+        <v>9.129741887643518E-14</v>
+      </c>
+      <c r="H8">
+        <v>1500</v>
+      </c>
+      <c r="I8">
+        <v>-2.755455298081545E-13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1500000</v>
+      </c>
+      <c r="G9">
+        <v>4500</v>
+      </c>
+      <c r="H9">
+        <v>-2.755455298081545E-13</v>
+      </c>
+      <c r="I9">
+        <v>3000000</v>
       </c>
     </row>
   </sheetData>
@@ -1093,7 +1513,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1101,32 +1521,47 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>100</v>
+        <v>259.807622554496</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>-25</v>
+        <v>5120</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>-20.83333333</v>
+        <v>-259.807622554496</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>0</v>
+        <v>450.0000004916132</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>-25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>20.83333333</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1136,7 +1571,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1144,62 +1579,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>-45.85662071797771</v>
+        <v>-20.00000000000002</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>-17.75673604907155</v>
+        <v>-3.413333333333336</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>136.0933672468462</v>
+        <v>-2560</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>100.0000000000018</v>
+        <v>-2.131628207280301E-14</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>-25</v>
+        <v>38.05434933333348</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>-20.83333332999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>-1.818989403545856E-12</v>
+        <v>1.4210854715202E-14</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>-25</v>
+        <v>4.973799150320701E-14</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>20.83333333000002</v>
+        <v>9.094947017729282E-13</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>-88.51278544571349</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>16.27237896450693</v>
+        <v>-34.64101600000015</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>-206.9613777127452</v>
+        <v>2.726541215025691E-12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>-9.999999999999991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>5.733165682073769E-29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>1.815103622959668E-12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>